<commit_message>
Añadido CSD a excel de notas y trabajo DCLAN Etapa 2 empezada
</commit_message>
<xml_diff>
--- a/3º/Notas_Tercero 2do Cuatri.xlsx
+++ b/3º/Notas_Tercero 2do Cuatri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ismael/Documents/GitHub/Ingenieria-Informatica/3º/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7BA674-E02F-7249-B15D-CA4C1C9A62A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F4E0308-2502-144F-81E3-A17A52FB9B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cuatri B" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
   <si>
     <t>Pract 1</t>
   </si>
@@ -250,6 +250,27 @@
   </si>
   <si>
     <t>Pract 9</t>
+  </si>
+  <si>
+    <t>CSD</t>
+  </si>
+  <si>
+    <t>Lab1</t>
+  </si>
+  <si>
+    <t>Lab2</t>
+  </si>
+  <si>
+    <t>Seguimiento 1</t>
+  </si>
+  <si>
+    <t>Seguimiento 2</t>
+  </si>
+  <si>
+    <t>Seguimiento 3</t>
+  </si>
+  <si>
+    <t>Seguimiento 4</t>
   </si>
 </sst>
 </file>
@@ -259,7 +280,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -313,13 +334,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -346,7 +360,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="32">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,6 +527,24 @@
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.14999847407452621"/>
         <bgColor rgb="FF999999"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FF9191FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FFB0B0FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FFD699FF"/>
       </patternFill>
     </fill>
   </fills>
@@ -590,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -608,9 +640,6 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -668,7 +697,7 @@
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -676,47 +705,47 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -738,17 +767,34 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -784,6 +830,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FF3CFA3C"/>
           <bgColor rgb="FF3CFA3C"/>
         </patternFill>
@@ -800,16 +854,16 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF6262"/>
-          <bgColor rgb="FFFF6262"/>
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
+          <fgColor rgb="FFFF6262"/>
+          <bgColor rgb="FFFF6262"/>
         </patternFill>
       </fill>
     </dxf>
@@ -825,6 +879,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF89CFF0"/>
       <color rgb="FFF8B068"/>
       <color rgb="FFFAC898"/>
       <color rgb="FFFBD9B7"/>
@@ -834,7 +889,6 @@
       <color rgb="FFFFB0B0"/>
       <color rgb="FFD3EDF9"/>
       <color rgb="FFC1E6F7"/>
-      <color rgb="FF89CFF0"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1046,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2091A348-E77A-4494-95CF-21AA3577EFE8}">
-  <dimension ref="A1:AF30"/>
+  <dimension ref="A1:AF41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="69" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="103" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1075,64 +1129,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="O1" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="9" t="s">
         <v>4</v>
       </c>
       <c r="U1" s="4"/>
@@ -1149,50 +1203,50 @@
       <c r="AF1" s="4"/>
     </row>
     <row r="2" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="30">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="29">
         <f>((B2+C2+D2+E2)/4)*0.1</f>
         <v>0</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="27">
         <v>5.56</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="27">
         <v>7.33</v>
       </c>
-      <c r="I2" s="28">
+      <c r="I2" s="27">
         <v>10</v>
       </c>
-      <c r="J2" s="28">
+      <c r="J2" s="27">
         <v>6.44</v>
       </c>
-      <c r="K2" s="28">
+      <c r="K2" s="27">
         <v>10</v>
       </c>
-      <c r="L2" s="30">
+      <c r="L2" s="29">
         <f>((G2+H2+I2+J2+K2+G4+H4+I4+J4+K4+G6+H6+I6)/13)*0.2</f>
         <v>0.60507692307692307</v>
       </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="30">
+      <c r="M2" s="28"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="29">
         <f>((M2+N2)/2)*0.2</f>
         <v>0</v>
       </c>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="28"/>
-      <c r="R2" s="28"/>
-      <c r="S2" s="30">
+      <c r="P2" s="28"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="29">
         <f>(((P2+Q2)/2)*0.4)+(R2*0.1)</f>
         <v>0</v>
       </c>
-      <c r="T2" s="51">
+      <c r="T2" s="50">
         <f>F2+L2+O2+S2</f>
         <v>0.60507692307692307</v>
       </c>
@@ -1210,30 +1264,30 @@
       <c r="AF2" s="4"/>
     </row>
     <row r="3" spans="1:32" ht="25.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="26" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
@@ -1254,20 +1308,20 @@
       <c r="AF3" s="3"/>
     </row>
     <row r="4" spans="1:32" ht="25.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
@@ -1288,13 +1342,13 @@
       <c r="AF4" s="3"/>
     </row>
     <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="25" t="s">
         <v>69</v>
       </c>
       <c r="U5" s="4"/>
@@ -1311,9 +1365,9 @@
       <c r="AF5" s="4"/>
     </row>
     <row r="6" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
@@ -1356,43 +1410,43 @@
       <c r="AF8" s="3"/>
     </row>
     <row r="9" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="32" t="s">
+      <c r="H9" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="32" t="s">
+      <c r="I9" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="32" t="s">
+      <c r="K9" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="M9" s="8" t="s">
         <v>4</v>
       </c>
       <c r="N9" s="5"/>
@@ -1416,38 +1470,40 @@
       <c r="AF9" s="4"/>
     </row>
     <row r="10" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="34">
+      <c r="B10" s="32"/>
+      <c r="C10" s="33">
         <f>B10*0.35</f>
         <v>0</v>
       </c>
-      <c r="D10" s="52">
+      <c r="D10" s="51">
         <v>10</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="32">
         <v>8</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="32">
         <v>8</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="34">
+      <c r="G10" s="32">
+        <v>8</v>
+      </c>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="33">
         <f>(D10*0.05)+(E10*0.1)+(F10*0.1)+(G10*0.05)+(H10*0.1)+(I10*0.15)</f>
-        <v>2.1</v>
-      </c>
-      <c r="K10" s="33"/>
-      <c r="L10" s="34">
+        <v>2.5</v>
+      </c>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33">
         <f>K10*0.1</f>
         <v>0</v>
       </c>
-      <c r="M10" s="35">
+      <c r="M10" s="34">
         <f>C10+J10+L10</f>
-        <v>2.1</v>
+        <v>2.5</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="4"/>
@@ -1470,20 +1526,20 @@
       <c r="AF10" s="4"/>
     </row>
     <row r="11" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -1504,20 +1560,20 @@
       <c r="AF11" s="3"/>
     </row>
     <row r="12" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
@@ -1538,64 +1594,64 @@
       <c r="AF12" s="3"/>
     </row>
     <row r="13" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G13" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="36" t="s">
+      <c r="H13" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="I13" s="36" t="s">
+      <c r="I13" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="13" t="s">
+      <c r="J13" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="36" t="s">
+      <c r="K13" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="L13" s="36" t="s">
+      <c r="L13" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="M13" s="36" t="s">
+      <c r="M13" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="N13" s="36" t="s">
+      <c r="N13" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="O13" s="36" t="s">
+      <c r="O13" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="P13" s="36" t="s">
+      <c r="P13" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="Q13" s="36" t="s">
+      <c r="Q13" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="R13" s="36" t="s">
+      <c r="R13" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="S13" s="13" t="s">
+      <c r="S13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="T13" s="13" t="s">
+      <c r="T13" s="12" t="s">
         <v>4</v>
       </c>
       <c r="U13" s="4"/>
@@ -1612,49 +1668,51 @@
       <c r="AF13" s="4"/>
     </row>
     <row r="14" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="36">
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="35">
         <f>(B14*0.35)+(C14*0.25)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E14" s="36">
         <v>13.75</v>
       </c>
-      <c r="F14" s="37">
+      <c r="F14" s="36">
         <v>14</v>
       </c>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="36">
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="35">
         <f>((E14+F14+G14+H14+I14)/5)*0.2</f>
         <v>1.1100000000000001</v>
       </c>
-      <c r="K14" s="37">
+      <c r="K14" s="36">
         <v>0</v>
       </c>
-      <c r="L14" s="37">
+      <c r="L14" s="36">
         <v>7</v>
       </c>
-      <c r="M14" s="37">
+      <c r="M14" s="36">
         <v>6.5</v>
       </c>
-      <c r="N14" s="37"/>
-      <c r="O14" s="37"/>
-      <c r="P14" s="37"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="36">
+      <c r="N14" s="36">
+        <v>6</v>
+      </c>
+      <c r="O14" s="36"/>
+      <c r="P14" s="36"/>
+      <c r="Q14" s="36"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="35">
         <f>((K14+L14+M14+N14+O14+P14+Q14+R14)/8)*0.2</f>
-        <v>0.33750000000000002</v>
-      </c>
-      <c r="T14" s="42">
+        <v>0.48750000000000004</v>
+      </c>
+      <c r="T14" s="41">
         <f>D14+J14+S14</f>
-        <v>1.4475000000000002</v>
+        <v>1.5975000000000001</v>
       </c>
       <c r="U14" s="4"/>
       <c r="V14" s="4"/>
@@ -1670,20 +1728,20 @@
       <c r="AF14" s="4"/>
     </row>
     <row r="15" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="26"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
@@ -1704,20 +1762,20 @@
       <c r="AF15" s="3"/>
     </row>
     <row r="16" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
+      <c r="A16" s="26"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="26"/>
+      <c r="K16" s="26"/>
+      <c r="L16" s="26"/>
+      <c r="M16" s="26"/>
+      <c r="N16" s="26"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
@@ -1738,42 +1796,42 @@
       <c r="AF16" s="3"/>
     </row>
     <row r="17" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="38" t="s">
+      <c r="E17" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F17" s="38" t="s">
+      <c r="F17" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="38" t="s">
+      <c r="H17" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="38" t="s">
+      <c r="I17" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="J17" s="14" t="s">
+      <c r="J17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="14" t="s">
+      <c r="K17" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
@@ -1793,36 +1851,36 @@
       <c r="AF17" s="4"/>
     </row>
     <row r="18" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="40">
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="39">
         <f>(B18*0.3)+(C18*0.3)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="39">
+      <c r="E18" s="38">
         <v>4.12</v>
       </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="40">
+      <c r="F18" s="38"/>
+      <c r="G18" s="39">
         <f>(E18*0.1)+(F18*0.1)</f>
         <v>0.41200000000000003</v>
       </c>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="41">
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="40">
         <f>(H18*0.1)+(I18*0.1)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="42">
+      <c r="K18" s="41">
         <f>D18+G18+J18</f>
         <v>0.41200000000000003</v>
       </c>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
+      <c r="L18" s="26"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
@@ -1842,20 +1900,20 @@
       <c r="AF18" s="4"/>
     </row>
     <row r="19" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="43"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
@@ -1876,20 +1934,20 @@
       <c r="AF19" s="3"/>
     </row>
     <row r="20" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3"/>
@@ -1910,43 +1968,43 @@
       <c r="AF20" s="3"/>
     </row>
     <row r="21" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E21" s="44" t="s">
+      <c r="E21" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="44" t="s">
+      <c r="G21" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="44" t="s">
+      <c r="H21" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="I21" s="44" t="s">
+      <c r="I21" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="J21" s="44" t="s">
+      <c r="J21" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="K21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L21" s="11" t="s">
+      <c r="L21" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="27"/>
+      <c r="M21" s="26"/>
       <c r="N21" s="5"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
@@ -1968,30 +2026,30 @@
       <c r="AF21" s="4"/>
     </row>
     <row r="22" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="45"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="44">
+      <c r="B22" s="44"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="43">
         <f>(B22*0.25)+(C22*0.25)</f>
         <v>0</v>
       </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="44">
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="43">
         <f>(E22*0.15)+(((F22+G22+H22+I22+J22)/5)*0.35)</f>
         <v>0</v>
       </c>
-      <c r="L22" s="47">
+      <c r="L22" s="46">
         <f>D22+K22</f>
         <v>0</v>
       </c>
-      <c r="M22" s="27"/>
+      <c r="M22" s="26"/>
       <c r="N22" s="5"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
@@ -2013,20 +2071,20 @@
       <c r="AF22" s="4"/>
     </row>
     <row r="23" spans="1:32" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="43"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
@@ -2047,20 +2105,20 @@
       <c r="AF23" s="3"/>
     </row>
     <row r="24" spans="1:32" ht="13.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -2081,43 +2139,43 @@
       <c r="AF24" s="3"/>
     </row>
     <row r="25" spans="1:32" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="48" t="s">
+      <c r="B25" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="48" t="s">
+      <c r="F25" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="48" t="s">
+      <c r="H25" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="I25" s="48" t="s">
+      <c r="I25" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="J25" s="48" t="s">
+      <c r="J25" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="K25" s="12" t="s">
+      <c r="K25" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="L25" s="12" t="s">
+      <c r="L25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="M25" s="27"/>
+      <c r="M25" s="26"/>
       <c r="N25" s="5"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
@@ -2139,33 +2197,33 @@
       <c r="AF25" s="4"/>
     </row>
     <row r="26" spans="1:32" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="48">
+      <c r="B26" s="48"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="47">
         <f>(B26*0.3)+(C26*0.1)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="48">
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="47">
         <f>(E26*0.1)+(F26*0.2)</f>
         <v>0</v>
       </c>
-      <c r="H26" s="49"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="49"/>
-      <c r="K26" s="48">
+      <c r="H26" s="48"/>
+      <c r="I26" s="48"/>
+      <c r="J26" s="48"/>
+      <c r="K26" s="47">
         <f>(H26*0.1)+(I26*0.1)+(J26*0.1)</f>
         <v>0</v>
       </c>
-      <c r="L26" s="50">
+      <c r="L26" s="49">
         <f>D26+G26+K26</f>
         <v>0</v>
       </c>
-      <c r="M26" s="27"/>
+      <c r="M26" s="26"/>
       <c r="N26" s="5"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
@@ -2182,12 +2240,14 @@
       <c r="AA26" s="1"/>
       <c r="AB26" s="2"/>
       <c r="AC26" s="2"/>
-      <c r="AD26" s="2"/>
+      <c r="AD26" s="2">
+        <v>6</v>
+      </c>
       <c r="AE26" s="2"/>
       <c r="AF26" s="2"/>
     </row>
     <row r="27" spans="1:32" ht="14" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2230,32 +2290,46 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="1:32" ht="24" x14ac:dyDescent="0.2">
-      <c r="A29" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="7"/>
+    <row r="29" spans="1:32" ht="19" x14ac:dyDescent="0.15">
+      <c r="A29" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="F29" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="I29" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="J29" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="K29" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" s="54" t="s">
+        <v>4</v>
+      </c>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
@@ -2264,39 +2338,38 @@
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
     </row>
-    <row r="30" spans="1:32" ht="24" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="24">
-        <f>T2</f>
-        <v>0.60507692307692307</v>
-      </c>
-      <c r="C30" s="24">
-        <f>M10</f>
-        <v>2.1</v>
-      </c>
-      <c r="D30" s="24">
-        <f>T14</f>
-        <v>1.4475000000000002</v>
-      </c>
-      <c r="E30" s="24">
-        <f>K18</f>
-        <v>0.41200000000000003</v>
-      </c>
-      <c r="F30" s="24">
-        <f>L22</f>
+    <row r="30" spans="1:32" ht="19" x14ac:dyDescent="0.15">
+      <c r="A30" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="48">
+        <v>5.38</v>
+      </c>
+      <c r="C30" s="48"/>
+      <c r="D30" s="47">
+        <f>(B30*0.3)+(C30*0.3)</f>
+        <v>1.6139999999999999</v>
+      </c>
+      <c r="E30" s="48">
+        <v>10</v>
+      </c>
+      <c r="F30" s="48"/>
+      <c r="G30" s="47">
+        <f>(E30*0.15)+(F30*0.15)</f>
+        <v>1.5</v>
+      </c>
+      <c r="H30" s="48"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="47">
+        <f>(I30*0.1)+(J30*0.1)+(K30*0.1)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="24">
-        <f>L26</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="25">
-        <f>(B30+C30+D30+E30+F30+G30)/6</f>
-        <v>0.76076282051282051</v>
-      </c>
-      <c r="I30" s="7"/>
+      <c r="M30" s="46">
+        <f>D30+G30+L30</f>
+        <v>3.1139999999999999</v>
+      </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
@@ -2305,41 +2378,108 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
     </row>
+    <row r="40" spans="1:8" ht="24" x14ac:dyDescent="0.15">
+      <c r="A40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="24" x14ac:dyDescent="0.15">
+      <c r="A41" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="23">
+        <f>T2</f>
+        <v>0.60507692307692307</v>
+      </c>
+      <c r="C41" s="23">
+        <f>M10</f>
+        <v>2.5</v>
+      </c>
+      <c r="D41" s="23">
+        <f>T14</f>
+        <v>1.5975000000000001</v>
+      </c>
+      <c r="E41" s="23">
+        <f>K18</f>
+        <v>0.41200000000000003</v>
+      </c>
+      <c r="F41" s="23">
+        <f>L22</f>
+        <v>0</v>
+      </c>
+      <c r="G41" s="23">
+        <f>L26</f>
+        <v>0</v>
+      </c>
+      <c r="H41" s="24">
+        <f>(B41+C41+D41+E41+F41+G41)/6</f>
+        <v>0.85242948717948719</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="9" type="noConversion"/>
-  <conditionalFormatting sqref="B30:G30">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="B41:G41">
+    <cfRule type="cellIs" dxfId="10" priority="7" operator="greaterThan">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H41">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
       <formula>5</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H30">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
-      <formula>5</formula>
-    </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="4" priority="4">
-      <formula>LEN(TRIM(H30))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="6" priority="6">
+      <formula>LEN(TRIM(H41))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2 M10 K18 L22 L26">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="greaterThanOrEqual">
       <formula>9</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="lessThan">
-      <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T14">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+      <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThanOrEqual">
       <formula>9</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M30">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>5</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
+      <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Añadido ETC a excel y submission ETC
</commit_message>
<xml_diff>
--- a/3º/Notas_Tercero 2do Cuatri.xlsx
+++ b/3º/Notas_Tercero 2do Cuatri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Ingenieria-Informatica\3º\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C74A97-0682-4608-84E6-EC46AE460131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B030879-D0DF-45B6-AA13-D5BF4D5A7CA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="90">
   <si>
     <t>Pract 1</t>
   </si>
@@ -271,6 +271,42 @@
   </si>
   <si>
     <t>Seguimiento 4</t>
+  </si>
+  <si>
+    <t>ETC</t>
+  </si>
+  <si>
+    <t>Parcial 3</t>
+  </si>
+  <si>
+    <t>Parcial 4</t>
+  </si>
+  <si>
+    <t>Total Parciales</t>
+  </si>
+  <si>
+    <t>Eval 1</t>
+  </si>
+  <si>
+    <t>Eval 2</t>
+  </si>
+  <si>
+    <t>Eval 3</t>
+  </si>
+  <si>
+    <t>Eval 4</t>
+  </si>
+  <si>
+    <t>Eval 5</t>
+  </si>
+  <si>
+    <t>Total Practicas</t>
+  </si>
+  <si>
+    <t>No presencial</t>
+  </si>
+  <si>
+    <t>Nota final</t>
   </si>
 </sst>
 </file>
@@ -280,7 +316,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -359,8 +395,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="32">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +588,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FFD699FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor rgb="FF9191FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor rgb="FF9191FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -622,7 +689,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -782,6 +849,14 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1103,7 +1178,7 @@
   <dimension ref="A1:AF41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2388,7 +2463,92 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="40" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" s="57" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="57" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="57" t="s">
+        <v>80</v>
+      </c>
+      <c r="F34" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34" s="57" t="s">
+        <v>82</v>
+      </c>
+      <c r="H34" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="I34" s="57" t="s">
+        <v>84</v>
+      </c>
+      <c r="J34" s="57" t="s">
+        <v>85</v>
+      </c>
+      <c r="K34" s="57" t="s">
+        <v>86</v>
+      </c>
+      <c r="L34" s="57" t="s">
+        <v>87</v>
+      </c>
+      <c r="M34" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="N34" s="57" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="58">
+        <v>5.6</v>
+      </c>
+      <c r="C35" s="58">
+        <v>4.7</v>
+      </c>
+      <c r="D35" s="58">
+        <v>4.75</v>
+      </c>
+      <c r="E35" s="58"/>
+      <c r="F35" s="58">
+        <f>B35*0.15+C35*0.2+D35*0.15+E35*0.2</f>
+        <v>2.4925000000000002</v>
+      </c>
+      <c r="G35" s="58">
+        <v>8.67</v>
+      </c>
+      <c r="H35" s="58">
+        <v>5.2</v>
+      </c>
+      <c r="I35" s="58">
+        <v>7.25</v>
+      </c>
+      <c r="J35" s="58">
+        <v>3.17</v>
+      </c>
+      <c r="K35" s="58"/>
+      <c r="L35" s="58">
+        <f>(G35*0.25+H35*0.18+I35*0.07+J35*0.25+K35*0.25)*0.25</f>
+        <v>1.1008749999999998</v>
+      </c>
+      <c r="M35" s="58"/>
+      <c r="N35" s="58">
+        <f>F35+L35+M35</f>
+        <v>3.593375</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
         <v>12</v>
       </c>
@@ -2414,7 +2574,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Update de notas ADS-ETC-DCE
</commit_message>
<xml_diff>
--- a/3º/Notas_Tercero 2do Cuatri.xlsx
+++ b/3º/Notas_Tercero 2do Cuatri.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Ingenieria-Informatica\3º\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EBF341-70D9-4943-B2F8-91D07F14ADAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B9181D-7508-4C20-B2B4-7E04DEBB975D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1177,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2091A348-E77A-4494-95CF-21AA3577EFE8}">
   <dimension ref="A1:AF41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H52" sqref="H52"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1577,14 +1577,16 @@
         <f>(D10*0.05)+(E10*0.1)+(F10*0.1)+(G10*0.05)+(H10*0.1)+(I10*0.15)</f>
         <v>4.7100000000000009</v>
       </c>
-      <c r="K10" s="32"/>
+      <c r="K10" s="32">
+        <v>8.8000000000000007</v>
+      </c>
       <c r="L10" s="33">
         <f>K10*0.1</f>
-        <v>0</v>
+        <v>0.88000000000000012</v>
       </c>
       <c r="M10" s="34">
         <f>C10+J10+L10</f>
-        <v>6.74</v>
+        <v>7.62</v>
       </c>
       <c r="N10" s="5"/>
       <c r="O10" s="4"/>
@@ -1962,10 +1964,12 @@
       <c r="E18" s="38">
         <v>4.12</v>
       </c>
-      <c r="F18" s="38"/>
+      <c r="F18" s="38">
+        <v>3.71</v>
+      </c>
       <c r="G18" s="39">
         <f>(E18*0.1)+(F18*0.1)</f>
-        <v>0.41200000000000003</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="H18" s="38">
         <v>9.9</v>
@@ -1979,7 +1983,7 @@
       </c>
       <c r="K18" s="41">
         <f>D18+G18+J18</f>
-        <v>2.302</v>
+        <v>2.673</v>
       </c>
       <c r="L18" s="26"/>
       <c r="M18" s="26"/>
@@ -2135,12 +2139,10 @@
       <c r="B22" s="44">
         <v>7.6</v>
       </c>
-      <c r="C22" s="45">
-        <v>2</v>
-      </c>
+      <c r="C22" s="45"/>
       <c r="D22" s="43">
         <f>(B22*0.25)+(C22*0.25)</f>
-        <v>2.4</v>
+        <v>1.9</v>
       </c>
       <c r="E22" s="45">
         <v>8.3000000000000007</v>
@@ -2151,18 +2153,16 @@
       <c r="G22" s="45">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H22" s="45">
-        <v>8</v>
-      </c>
+      <c r="H22" s="45"/>
       <c r="I22" s="45"/>
       <c r="J22" s="45"/>
       <c r="K22" s="43">
         <f>(E22*0.15)+(((F22+G22+H22+I22+J22)/5)*0.35)</f>
-        <v>3.1070000000000002</v>
+        <v>2.5470000000000002</v>
       </c>
       <c r="L22" s="46">
         <f>D22+K22</f>
-        <v>5.5069999999999997</v>
+        <v>4.4470000000000001</v>
       </c>
       <c r="M22" s="26"/>
       <c r="N22" s="5"/>
@@ -2478,12 +2478,11 @@
       <c r="J30" s="48"/>
       <c r="K30" s="48"/>
       <c r="L30" s="47">
-        <f>(I30*0.1)+(J30*0.1)+(K30*0.1)</f>
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="M30" s="46">
         <f>D30+G30+L30</f>
-        <v>3.1470000000000002</v>
+        <v>3.4970000000000003</v>
       </c>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -2620,7 +2619,7 @@
       </c>
       <c r="C41" s="23">
         <f>M10</f>
-        <v>6.74</v>
+        <v>7.62</v>
       </c>
       <c r="D41" s="23">
         <f>T14</f>
@@ -2628,19 +2627,19 @@
       </c>
       <c r="E41" s="23">
         <f>K18</f>
-        <v>2.302</v>
+        <v>2.673</v>
       </c>
       <c r="F41" s="23">
         <f>L22</f>
-        <v>5.5069999999999997</v>
+        <v>4.4470000000000001</v>
       </c>
       <c r="G41" s="23">
         <f>M30</f>
-        <v>3.1470000000000002</v>
+        <v>3.4970000000000003</v>
       </c>
       <c r="H41" s="24">
         <f>(B41+C41+D41+E41+F41+G41)/6</f>
-        <v>4.9233125000000006</v>
+        <v>5.0134791666666674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Notas_Tercero 2do Cuatri.xlsx
Ultimas notas 2do Cuatri 3º
</commit_message>
<xml_diff>
--- a/3º/Notas_Tercero 2do Cuatri.xlsx
+++ b/3º/Notas_Tercero 2do Cuatri.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Ingenieria-Informatica\3º\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ismael/Documents/GitHub/Ingenieria-Informatica/3º/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFD8C13-C19A-4AD5-BC44-1721816D6FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F50BBF3-9F0F-ED42-A0C0-5F43E34CFDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cuatri B" sheetId="2" r:id="rId1"/>
@@ -1071,29 +1071,29 @@
   <dimension ref="A1:AF32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29.5" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" customWidth="1"/>
+    <col min="7" max="7" width="24.5" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="27.140625" customWidth="1"/>
-    <col min="10" max="10" width="25.42578125" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
-    <col min="12" max="12" width="25.42578125" customWidth="1"/>
-    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" customWidth="1"/>
+    <col min="10" max="10" width="25.5" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="25.5" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" customWidth="1"/>
     <col min="14" max="14" width="30" customWidth="1"/>
-    <col min="15" max="15" width="26.42578125" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" customWidth="1"/>
-    <col min="17" max="17" width="21.140625" customWidth="1"/>
-    <col min="18" max="18" width="19.28515625" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" customWidth="1"/>
-    <col min="20" max="20" width="17.42578125" customWidth="1"/>
+    <col min="15" max="15" width="26.5" customWidth="1"/>
+    <col min="16" max="16" width="20.5" customWidth="1"/>
+    <col min="17" max="17" width="21.1640625" customWidth="1"/>
+    <col min="18" max="18" width="19.33203125" customWidth="1"/>
+    <col min="19" max="19" width="21.83203125" customWidth="1"/>
+    <col min="20" max="20" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1156,7 +1156,7 @@
       <c r="AE1" s="4"/>
       <c r="AF1" s="4"/>
     </row>
-    <row r="2" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -1220,7 +1220,7 @@
       <c r="AE2" s="4"/>
       <c r="AF2" s="4"/>
     </row>
-    <row r="3" spans="1:32" ht="25.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" ht="25.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -1328,7 +1328,7 @@
       <c r="AE4" s="4"/>
       <c r="AF4" s="4"/>
     </row>
-    <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
@@ -1406,7 +1406,7 @@
       <c r="AE5" s="4"/>
       <c r="AF5" s="4"/>
     </row>
-    <row r="6" spans="1:32" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="24"/>
       <c r="C6" s="24"/>
@@ -1440,7 +1440,7 @@
       <c r="AE6" s="3"/>
       <c r="AF6" s="3"/>
     </row>
-    <row r="7" spans="1:32" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
@@ -1474,7 +1474,7 @@
       <c r="AE7" s="3"/>
       <c r="AF7" s="3"/>
     </row>
-    <row r="8" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>44</v>
       </c>
@@ -1529,7 +1529,7 @@
       <c r="AE8" s="4"/>
       <c r="AF8" s="4"/>
     </row>
-    <row r="9" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
@@ -1588,7 +1588,7 @@
       <c r="AE9" s="4"/>
       <c r="AF9" s="4"/>
     </row>
-    <row r="10" spans="1:32" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="36"/>
       <c r="B10" s="24"/>
       <c r="C10" s="24"/>
@@ -1622,7 +1622,7 @@
       <c r="AE10" s="3"/>
       <c r="AF10" s="3"/>
     </row>
-    <row r="11" spans="1:32" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="24"/>
       <c r="C11" s="24"/>
@@ -1656,7 +1656,7 @@
       <c r="AE11" s="3"/>
       <c r="AF11" s="3"/>
     </row>
-    <row r="12" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>17</v>
       </c>
@@ -1714,7 +1714,7 @@
       <c r="AE12" s="4"/>
       <c r="AF12" s="4"/>
     </row>
-    <row r="13" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>5</v>
       </c>
@@ -1725,8 +1725,8 @@
         <v>0.6</v>
       </c>
       <c r="D13" s="37">
-        <f>(B13*0.25)+(C13*0.25)</f>
-        <v>2.0499999999999998</v>
+        <f>(B13*0.3)+(C13*0.2)</f>
+        <v>2.4</v>
       </c>
       <c r="E13" s="39">
         <v>8.3000000000000007</v>
@@ -1748,7 +1748,7 @@
       </c>
       <c r="L13" s="40">
         <f>D13+K13</f>
-        <v>5.2492599999999996</v>
+        <v>5.5992600000000001</v>
       </c>
       <c r="M13" s="24"/>
       <c r="N13" s="5"/>
@@ -1771,7 +1771,7 @@
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
     </row>
-    <row r="14" spans="1:32" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="24"/>
       <c r="C14" s="24"/>
@@ -1805,7 +1805,7 @@
       <c r="AE14" s="3"/>
       <c r="AF14" s="3"/>
     </row>
-    <row r="15" spans="1:32" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
@@ -1839,7 +1839,7 @@
       <c r="AE15" s="3"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>18</v>
       </c>
@@ -1897,7 +1897,7 @@
       <c r="AE16" s="4"/>
       <c r="AF16" s="4"/>
     </row>
-    <row r="17" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>5</v>
       </c>
@@ -1945,7 +1945,7 @@
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
     </row>
-    <row r="18" spans="1:32" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1979,7 +1979,7 @@
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
     </row>
-    <row r="19" spans="1:32" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -2073,7 +2073,7 @@
       <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
     </row>
-    <row r="21" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="45" t="s">
         <v>5</v>
       </c>
@@ -2128,7 +2128,7 @@
       <c r="AE21" s="4"/>
       <c r="AF21" s="4"/>
     </row>
-    <row r="22" spans="1:32" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="U22" s="1"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
@@ -2142,7 +2142,7 @@
       <c r="AE22" s="3"/>
       <c r="AF22" s="3"/>
     </row>
-    <row r="23" spans="1:32" ht="13.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:32" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
@@ -2155,7 +2155,7 @@
       <c r="AE23" s="3"/>
       <c r="AF23" s="3"/>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:32" ht="14" x14ac:dyDescent="0.15">
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
       <c r="X24" s="4"/>
@@ -2168,7 +2168,7 @@
       <c r="AE24" s="4"/>
       <c r="AF24" s="4"/>
     </row>
-    <row r="25" spans="1:32" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:32" ht="19" x14ac:dyDescent="0.15">
       <c r="A25" s="48" t="s">
         <v>60</v>
       </c>
@@ -2225,7 +2225,7 @@
       <c r="AE25" s="2"/>
       <c r="AF25" s="2"/>
     </row>
-    <row r="26" spans="1:32" ht="18.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:32" ht="19" x14ac:dyDescent="0.15">
       <c r="A26" s="49" t="s">
         <v>5</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>5.2008750000000008</v>
       </c>
     </row>
-    <row r="31" spans="1:32" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:32" ht="24" x14ac:dyDescent="0.15">
       <c r="A31" s="14" t="s">
         <v>11</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:32" ht="23.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:32" ht="24" x14ac:dyDescent="0.15">
       <c r="A32" s="21" t="s">
         <v>12</v>
       </c>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="F32" s="22">
         <f>L13</f>
-        <v>5.2492599999999996</v>
+        <v>5.5992600000000001</v>
       </c>
       <c r="G32" s="22">
         <f>M21</f>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="H32" s="23">
         <f>(B32+C32+D32+E32+F32+G32)/6</f>
-        <v>6.1234391666666665</v>
+        <v>6.1817725000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2352,19 +2352,19 @@
       <formula>LEN(TRIM(H32))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M21">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="M2 K9 L13 L17">
+    <cfRule type="cellIs" dxfId="5" priority="10" operator="lessThan">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="11" operator="greaterThanOrEqual">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2 K9 L13 L17">
-    <cfRule type="cellIs" dxfId="3" priority="10" operator="lessThan">
+  <conditionalFormatting sqref="M21">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThanOrEqual">
       <formula>9</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>